<commit_message>
sendt til alle. venter på savar
</commit_message>
<xml_diff>
--- a/Problembeskrivelser.xlsx
+++ b/Problembeskrivelser.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stian\OneDrive\Dokumenter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://hioa365-my.sharepoint.com/personal/rashasin_oslomet_no/Documents/Skrivebord/DIKU/DIKU-2/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{29B90277-8109-433C-A3FB-07749C8DF363}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="8_{29B90277-8109-433C-A3FB-07749C8DF363}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{D13B2DCF-ABEB-4912-BF11-452AA962AFA3}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{DC14DD5F-A07F-4B12-B39B-90ED859D2E8C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{DC14DD5F-A07F-4B12-B39B-90ED859D2E8C}"/>
   </bookViews>
   <sheets>
-    <sheet name="Business as usual" sheetId="1" r:id="rId1"/>
-    <sheet name="E-lab" sheetId="2" r:id="rId2"/>
-    <sheet name="Fygital" sheetId="3" r:id="rId3"/>
-    <sheet name="E-learning" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet1" sheetId="5" r:id="rId1"/>
+    <sheet name="Business as usual" sheetId="1" r:id="rId2"/>
+    <sheet name="E-learning" sheetId="4" r:id="rId3"/>
+    <sheet name="Fygital" sheetId="3" r:id="rId4"/>
+    <sheet name="E-lab" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -376,7 +377,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -671,25 +672,37 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB84041F-0C25-4177-BC28-4A1FD6B6A4DF}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{435B4456-F17C-42F1-A9BF-EA99E251F090}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="42" style="2" customWidth="1"/>
-    <col min="2" max="2" width="26.109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="26.140625" style="2" customWidth="1"/>
     <col min="3" max="3" width="30" style="2" customWidth="1"/>
-    <col min="4" max="4" width="20.44140625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="27.5546875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.5703125" style="2" customWidth="1"/>
     <col min="6" max="6" width="19" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="11.5546875" style="2"/>
+    <col min="7" max="16384" width="11.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>5</v>
       </c>
@@ -698,7 +711,7 @@
       <c r="D1" s="3"/>
       <c r="E1" s="3"/>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -718,7 +731,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>7</v>
       </c>
@@ -738,7 +751,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>8</v>
       </c>
@@ -758,7 +771,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>9</v>
       </c>
@@ -773,7 +786,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>10</v>
       </c>
@@ -786,7 +799,7 @@
       <c r="D6" s="4"/>
       <c r="E6" s="4"/>
     </row>
-    <row r="7" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>11</v>
       </c>
@@ -799,7 +812,7 @@
       <c r="D7" s="4"/>
       <c r="E7" s="4"/>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
         <v>12</v>
       </c>
@@ -812,7 +825,7 @@
       <c r="D8" s="4"/>
       <c r="E8" s="4"/>
     </row>
-    <row r="9" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9" s="4"/>
       <c r="B9" s="4" t="s">
         <v>29</v>
@@ -823,7 +836,7 @@
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="E14" s="2" t="s">
         <v>6</v>
       </c>
@@ -834,31 +847,30 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B08CF4-8E89-4ECE-B9D5-9E0AA5AD5C40}">
-  <dimension ref="A1:F7"/>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C173FB4E-4CC9-4139-8DF3-8011C21AA20C}">
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.44140625" style="2" customWidth="1"/>
-    <col min="2" max="2" width="23.33203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="21.109375" style="2" customWidth="1"/>
-    <col min="4" max="4" width="21.21875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="23.77734375" style="2" customWidth="1"/>
-    <col min="6" max="6" width="21.6640625" style="2" customWidth="1"/>
-    <col min="7" max="16384" width="11.5546875" style="2"/>
+    <col min="1" max="1" width="24.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="22.85546875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="23.140625" style="4" customWidth="1"/>
+    <col min="4" max="5" width="21.7109375" style="4" customWidth="1"/>
+    <col min="6" max="6" width="22" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="11.5703125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -874,77 +886,91 @@
       <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>30</v>
+        <v>66</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>34</v>
+        <v>64</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>35</v>
+        <v>65</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="100.8" x14ac:dyDescent="0.3">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>31</v>
+        <v>67</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>70</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="B5" s="4"/>
+        <v>85</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>71</v>
+      </c>
       <c r="C5" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-    </row>
-    <row r="6" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A6" s="4"/>
-      <c r="B6" s="4"/>
+        <v>63</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="C6" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="4"/>
-      <c r="B7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+        <v>73</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="4" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09665734-B07B-447C-89EA-424649410D23}">
   <dimension ref="A1:F7"/>
   <sheetViews>
@@ -952,23 +978,23 @@
       <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.21875" style="4" customWidth="1"/>
-    <col min="2" max="2" width="20.33203125" style="4" customWidth="1"/>
-    <col min="3" max="3" width="22.109375" style="4" customWidth="1"/>
-    <col min="4" max="4" width="22.88671875" style="4" customWidth="1"/>
-    <col min="5" max="5" width="25.33203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="18.109375" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="11.5546875" style="4"/>
+    <col min="1" max="1" width="21.28515625" style="4" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" style="4" customWidth="1"/>
+    <col min="3" max="3" width="22.140625" style="4" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="4" customWidth="1"/>
+    <col min="5" max="5" width="25.28515625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="18.140625" style="4" customWidth="1"/>
+    <col min="7" max="16384" width="11.5703125" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -988,7 +1014,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
         <v>42</v>
       </c>
@@ -1008,7 +1034,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
         <v>43</v>
       </c>
@@ -1028,7 +1054,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
         <v>44</v>
       </c>
@@ -1042,7 +1068,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>79</v>
       </c>
@@ -1053,7 +1079,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>45</v>
       </c>
@@ -1063,30 +1089,31 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C173FB4E-4CC9-4139-8DF3-8011C21AA20C}">
-  <dimension ref="A1:F8"/>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9B08CF4-8E89-4ECE-B9D5-9E0AA5AD5C40}">
+  <dimension ref="A1:F7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.6640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="22.88671875" style="4" customWidth="1"/>
-    <col min="3" max="3" width="23.109375" style="4" customWidth="1"/>
-    <col min="4" max="5" width="21.77734375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="22" style="4" customWidth="1"/>
-    <col min="7" max="16384" width="11.5546875" style="4"/>
+    <col min="1" max="1" width="26.42578125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="23.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.140625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="21.28515625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="23.7109375" style="2" customWidth="1"/>
+    <col min="6" max="6" width="21.7109375" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="11.5703125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>0</v>
       </c>
@@ -1102,84 +1129,70 @@
       <c r="E2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="1" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>66</v>
+        <v>30</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>64</v>
+        <v>34</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>60</v>
+        <v>32</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="F3" s="4" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>70</v>
+        <v>31</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>62</v>
+        <v>36</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>41</v>
       </c>
       <c r="F4" s="4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" ht="57.6" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>71</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B5" s="4"/>
       <c r="C5" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="72" x14ac:dyDescent="0.3">
-      <c r="A6" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>72</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
       <c r="C6" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A7" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>73</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A8" s="4" t="s">
-        <v>69</v>
-      </c>
+        <v>39</v>
+      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1187,6 +1200,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100397E437080B18A4386D453C9A9FA6939" ma:contentTypeVersion="2" ma:contentTypeDescription="Opprett et nytt dokument." ma:contentTypeScope="" ma:versionID="e15f3e224d8dd52f2b13909b615be202">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="6cdb2f02-6ea5-4b97-a175-fc1305aeb4c7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f879d4c43ed6cb24089376ac0a8c1ad7" ns3:_="">
     <xsd:import namespace="6cdb2f02-6ea5-4b97-a175-fc1305aeb4c7"/>
@@ -1318,22 +1346,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B40F329-9BEB-4230-BD0F-EB622D2FA1F5}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="6cdb2f02-6ea5-4b97-a175-fc1305aeb4c7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87F1E374-EDEC-4E68-8C12-4D7FDDCF5596}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E1DE7F2E-2DFE-40CB-A598-E6391C738850}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -1349,28 +1386,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{87F1E374-EDEC-4E68-8C12-4D7FDDCF5596}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1B40F329-9BEB-4230-BD0F-EB622D2FA1F5}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="6cdb2f02-6ea5-4b97-a175-fc1305aeb4c7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>